<commit_message>
plottet ICR ID 5 og 6 Cl, SO4 og Silica
</commit_message>
<xml_diff>
--- a/data/ICR/ICR_2_samlet.xlsx
+++ b/data/ICR/ICR_2_samlet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/ICR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{508007A1-6A38-40A3-BA45-E5053CFCC365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85756C5A-0C43-4F53-A166-0EA0C257987B}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{508007A1-6A38-40A3-BA45-E5053CFCC365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E588E547-932C-43BC-9E55-A272BAD50A8F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{926BA01D-7E05-4040-85F6-3A23D61AC3DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{926BA01D-7E05-4040-85F6-3A23D61AC3DF}"/>
   </bookViews>
   <sheets>
     <sheet name="ID 4" sheetId="2" r:id="rId1"/>
@@ -461,7 +461,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:J6"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842E334A-F76A-44FE-B5B5-AEE102F75B1D}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3:H6"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +828,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J5"/>
+      <selection activeCell="C2" sqref="C2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,12 +889,6 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>42.6</v>
-      </c>
-      <c r="D2">
-        <v>56.2</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -903,18 +897,6 @@
       <c r="B3">
         <v>1.5</v>
       </c>
-      <c r="C3">
-        <v>41.6</v>
-      </c>
-      <c r="D3">
-        <v>56.4</v>
-      </c>
-      <c r="I3">
-        <v>35</v>
-      </c>
-      <c r="J3">
-        <v>60</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -923,18 +905,6 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>43.8</v>
-      </c>
-      <c r="D4">
-        <v>53</v>
-      </c>
-      <c r="I4">
-        <v>37.4</v>
-      </c>
-      <c r="J4">
-        <v>61</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -943,18 +913,6 @@
       <c r="B5">
         <v>6.5</v>
       </c>
-      <c r="C5">
-        <v>46.4</v>
-      </c>
-      <c r="D5">
-        <v>49.4</v>
-      </c>
-      <c r="I5">
-        <v>39.6</v>
-      </c>
-      <c r="J5">
-        <v>62.6</v>
-      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -962,12 +920,6 @@
       </c>
       <c r="B6">
         <v>7.25</v>
-      </c>
-      <c r="C6">
-        <v>48.2</v>
-      </c>
-      <c r="D6">
-        <v>49.8</v>
       </c>
     </row>
   </sheetData>
@@ -980,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EB39FE-0B87-4D76-B4D3-FA229DA848B6}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>